<commit_message>
Changes in  Actions and Scripts. IndhuTestData Added
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="132" windowWidth="20100" windowHeight="8472"/>
+    <workbookView xWindow="0" yWindow="132" windowWidth="20100" windowHeight="8472" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>!@#$%^&amp;*()</t>
+  </si>
+  <si>
+    <t>oct21@yopmail.com</t>
+  </si>
+  <si>
+    <t>Hiindhu11@</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -506,14 +512,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
   </cols>
@@ -547,6 +553,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Personal Info Validation Scripts
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/indhul/Desktop/sample/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="132" windowWidth="20100" windowHeight="8472" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="13220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
     <sheet name="SignIn" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="MyAcc_PInfo" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t>Username</t>
   </si>
@@ -70,13 +80,214 @@
   </si>
   <si>
     <t>Hiindhu11@</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>myacc_pinfoedit@yopmail.com</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>newVerifyPassword</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>address2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>verifyEmail</t>
+  </si>
+  <si>
+    <t>phonenumber</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>birthMonth</t>
+  </si>
+  <si>
+    <t>Acme</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Qwerty!2345</t>
+  </si>
+  <si>
+    <t>Acmetools</t>
+  </si>
+  <si>
+    <t>123 plaza drive</t>
+  </si>
+  <si>
+    <t>no 45</t>
+  </si>
+  <si>
+    <t>07044</t>
+  </si>
+  <si>
+    <t>99509</t>
+  </si>
+  <si>
+    <t>Anchorage</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Verona</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>35172</t>
+  </si>
+  <si>
+    <t>Trafford</t>
+  </si>
+  <si>
+    <t>93433</t>
+  </si>
+  <si>
+    <t>Grover Beach</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>34785</t>
+  </si>
+  <si>
+    <t>Wildwood</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>33306</t>
+  </si>
+  <si>
+    <t>Wilton Manors</t>
+  </si>
+  <si>
+    <t>30087</t>
+  </si>
+  <si>
+    <t>Smoke Rise</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>50632</t>
+  </si>
+  <si>
+    <t>Garwin</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>01062</t>
+  </si>
+  <si>
+    <t>Florence</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>20851</t>
+  </si>
+  <si>
+    <t>Rockville</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>pinfoedited@yopmail.com</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Cabinet Maker</t>
+  </si>
+  <si>
+    <t>Carpentry Work</t>
+  </si>
+  <si>
+    <t>Concrete Contractor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +322,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -139,12 +356,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -203,12 +424,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -238,12 +459,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -450,16 +671,16 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -472,7 +693,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -483,7 +704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -491,7 +712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -510,21 +731,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +759,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -552,7 +773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -563,20 +784,286 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" customWidth="1"/>
+    <col min="12" max="12" width="25.5" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2">
+        <v>9898989898</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" t="s">
+        <v>83</v>
+      </c>
+      <c r="O3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
+        <v>62</v>
+      </c>
+      <c r="O9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" t="s">
+        <v>65</v>
+      </c>
+      <c r="O10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" t="s">
+        <v>68</v>
+      </c>
+      <c r="O11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Homepage, Categorypage, MenuSelection changes
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/indhul/Desktop/sample/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="13220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="20376" windowHeight="12816"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
   <si>
     <t>Username</t>
   </si>
@@ -281,13 +276,25 @@
   </si>
   <si>
     <t>Concrete Contractor</t>
+  </si>
+  <si>
+    <t>SingleSearch</t>
+  </si>
+  <si>
+    <t>BrandSearch</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>IPI INDUSTRIES-HND1.2-000ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +335,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.9"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -356,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -365,6 +379,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -670,17 +687,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -690,10 +708,14 @@
       <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -703,8 +725,14 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -712,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -733,14 +761,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
   </cols>
@@ -809,17 +837,17 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" customWidth="1"/>
-    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
     <col min="11" max="11" width="21.33203125" customWidth="1"/>
-    <col min="12" max="12" width="25.5" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" customWidth="1"/>
     <col min="13" max="13" width="19.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
My Account test Data editing
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/indhul/Desktop/sample/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="20376" windowHeight="12816"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="11300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
   <si>
     <t>Username</t>
   </si>
@@ -278,23 +283,50 @@
     <t>Concrete Contractor</t>
   </si>
   <si>
-    <t>SingleSearch</t>
-  </si>
-  <si>
-    <t>BrandSearch</t>
-  </si>
-  <si>
-    <t>Honda</t>
-  </si>
-  <si>
-    <t>IPI INDUSTRIES-HND1.2-000ID</t>
+    <t>Pinfo</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>Sirius</t>
+  </si>
+  <si>
+    <t>500 ghj street</t>
+  </si>
+  <si>
+    <t>no 99</t>
+  </si>
+  <si>
+    <t>abooknoaddr@yopmail.com</t>
+  </si>
+  <si>
+    <t>Main Account with orders</t>
+  </si>
+  <si>
+    <t>Account without Orders</t>
+  </si>
+  <si>
+    <t>Account for Editing Personal infor</t>
+  </si>
+  <si>
+    <t>Account with 0 address in the address book</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Edit values in Personal info</t>
+  </si>
+  <si>
+    <t>Revert back the values in personal info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,13 +367,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9.9"/>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -370,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -379,9 +404,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -687,18 +709,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.19921875" customWidth="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -708,14 +729,10 @@
       <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -725,14 +742,8 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -740,7 +751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -759,337 +770,398 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.3984375" customWidth="1"/>
+    <col min="2" max="2" width="28.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" customWidth="1"/>
-    <col min="12" max="12" width="25.44140625" customWidth="1"/>
-    <col min="13" max="13" width="19.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.19921875" customWidth="1"/>
+    <col min="4" max="4" width="17.19921875" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" customWidth="1"/>
+    <col min="10" max="10" width="10.19921875" customWidth="1"/>
+    <col min="11" max="11" width="12.3984375" customWidth="1"/>
+    <col min="12" max="12" width="21.3984375" customWidth="1"/>
+    <col min="13" max="13" width="25.3984375" customWidth="1"/>
+    <col min="14" max="14" width="19.59765625" customWidth="1"/>
+    <col min="15" max="15" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>36</v>
       </c>
       <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>38</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>45</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2">
         <v>9898989898</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>82</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H3" s="6" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>42</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>43</v>
       </c>
-      <c r="N3" t="s">
+      <c r="L3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <v>8877887788</v>
+      </c>
+      <c r="O3" t="s">
         <v>83</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H4" s="6" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>48</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>46</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>84</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H5" s="6" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>50</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>51</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H6" s="6" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>53</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>54</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H7" s="6" t="s">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>56</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>54</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H8" s="6" t="s">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>58</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>59</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H9" s="6" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>61</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>62</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H10" s="6" t="s">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I10" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>64</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>65</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H11" s="6" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>67</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>68</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O12" t="s">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O13" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P13" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="L2" r:id="rId2"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="M2" r:id="rId2"/>
+    <hyperlink ref="L3" r:id="rId3"/>
+    <hyperlink ref="M3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Till Coupons Page Actions
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20700" windowHeight="12150" activeTab="3"/>
+    <workbookView windowWidth="20430" windowHeight="11595" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
     <sheet name="SignIn" sheetId="2" r:id="rId2"/>
     <sheet name="MyAcc_PInfo" sheetId="3" r:id="rId3"/>
     <sheet name="addrBook" sheetId="4" r:id="rId4"/>
+    <sheet name="creditCardInfo" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119">
   <si>
     <t>SearchSKU</t>
   </si>
@@ -73,10 +74,7 @@
     <t>Account without Orders</t>
   </si>
   <si>
-    <t>oct21@yopmail.com</t>
-  </si>
-  <si>
-    <t>Hiindhu11@</t>
+    <t>acmenoorders@yopmail.com</t>
   </si>
   <si>
     <t>Type a logon ID in the Logon ID field.</t>
@@ -338,6 +336,45 @@
   </si>
   <si>
     <t>newshipemail@yopmail.com</t>
+  </si>
+  <si>
+    <t>PaymentMethod</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>ExpMonth</t>
+  </si>
+  <si>
+    <t>ExpYear</t>
+  </si>
+  <si>
+    <t>New Credit card info to be added in the My Account</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>mccBillingfname</t>
+  </si>
+  <si>
+    <t>mccBillinglname</t>
+  </si>
+  <si>
+    <t>228 Park Ave S</t>
+  </si>
+  <si>
+    <t>verona</t>
+  </si>
+  <si>
+    <t>mccbillemail@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -345,12 +382,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -372,6 +409,13 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color indexed="12"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -389,6 +433,25 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -404,18 +467,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -431,6 +482,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -441,30 +530,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -485,6 +551,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -492,50 +580,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -552,6 +596,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -576,84 +626,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -661,78 +777,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,6 +787,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -781,30 +840,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -829,17 +864,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -848,176 +892,180 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1410,7 +1458,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A6"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1420,17 +1468,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -1439,7 +1487,7 @@
       <c r="B2">
         <v>5</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1475,7 +1523,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -1488,19 +1536,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1508,16 +1556,16 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1525,22 +1573,22 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -1548,16 +1596,21 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="acmeautomation1@yopmail.com"/>
+    <hyperlink ref="B5" r:id="rId2" display="abooknoaddr@yopmail.com"/>
+    <hyperlink ref="B3" r:id="rId3" display="acmenoorders@yopmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
@@ -1570,7 +1623,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15"/>
@@ -1588,276 +1641,276 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" t="s">
         <v>48</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>50</v>
+      <c r="M2" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="N2">
         <v>9898989898</v>
       </c>
       <c r="O2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" t="s">
         <v>51</v>
-      </c>
-      <c r="P2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>56</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>57</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" t="s">
         <v>59</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>60</v>
       </c>
-      <c r="K3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>22</v>
+      <c r="L3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="N3">
         <v>8877887788</v>
       </c>
       <c r="O3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P3" t="s">
         <v>62</v>
       </c>
-      <c r="P3" t="s">
+    </row>
+    <row r="4" spans="9:16">
+      <c r="I4" s="9" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="9:16">
-      <c r="I4" s="7" t="s">
+      <c r="J4" t="s">
         <v>64</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>65</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
         <v>66</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>67</v>
       </c>
-      <c r="P4" t="s">
+    </row>
+    <row r="5" spans="9:16">
+      <c r="I5" s="9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="9:16">
-      <c r="I5" s="7" t="s">
+      <c r="J5" t="s">
         <v>69</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>70</v>
       </c>
-      <c r="K5" t="s">
+      <c r="P5" t="s">
         <v>71</v>
       </c>
-      <c r="P5" t="s">
+    </row>
+    <row r="6" spans="9:16">
+      <c r="I6" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="9:16">
-      <c r="I6" s="7" t="s">
+      <c r="J6" t="s">
         <v>73</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>74</v>
       </c>
-      <c r="K6" t="s">
+      <c r="P6" t="s">
         <v>75</v>
       </c>
-      <c r="P6" t="s">
+    </row>
+    <row r="7" spans="9:16">
+      <c r="I7" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="9:16">
-      <c r="I7" s="7" t="s">
+      <c r="J7" t="s">
         <v>77</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" t="s">
         <v>78</v>
       </c>
-      <c r="K7" t="s">
-        <v>75</v>
-      </c>
-      <c r="P7" t="s">
+    </row>
+    <row r="8" spans="9:16">
+      <c r="I8" s="9" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="9:16">
-      <c r="I8" s="7" t="s">
+      <c r="J8" t="s">
         <v>80</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>81</v>
       </c>
-      <c r="K8" t="s">
+      <c r="P8" t="s">
         <v>82</v>
       </c>
-      <c r="P8" t="s">
+    </row>
+    <row r="9" spans="9:16">
+      <c r="I9" s="9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="9:16">
-      <c r="I9" s="7" t="s">
+      <c r="J9" t="s">
         <v>84</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>85</v>
       </c>
-      <c r="K9" t="s">
+      <c r="P9" t="s">
         <v>86</v>
       </c>
-      <c r="P9" t="s">
+    </row>
+    <row r="10" spans="9:16">
+      <c r="I10" s="9" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="9:16">
-      <c r="I10" s="7" t="s">
+      <c r="J10" t="s">
         <v>88</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>89</v>
       </c>
-      <c r="K10" t="s">
+      <c r="P10" t="s">
         <v>90</v>
       </c>
-      <c r="P10" t="s">
+    </row>
+    <row r="11" spans="9:16">
+      <c r="I11" s="9" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="9:16">
-      <c r="I11" s="7" t="s">
+      <c r="J11" t="s">
         <v>92</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>93</v>
       </c>
-      <c r="K11" t="s">
+      <c r="P11" t="s">
         <v>94</v>
-      </c>
-      <c r="P11" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="12" spans="16:16">
       <c r="P12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="16:16">
       <c r="P13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1878,93 +1931,93 @@
   <sheetPr/>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.2857142857143" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="16380" width="23.2857142857143" style="1" customWidth="1"/>
-    <col min="16381" max="16384" width="23.2857142857143" style="1"/>
+    <col min="1" max="16380" width="23.2857142857143" style="2" customWidth="1"/>
+    <col min="16381" max="16384" width="23.2857142857143" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" ht="30" spans="1:12">
+      <c r="A2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" ht="30" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L2" s="1">
+      <c r="L2" s="2">
         <v>5566556655</v>
       </c>
     </row>
@@ -1975,4 +2028,123 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="24.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="19.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="19.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="13.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="16.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="20.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="22.2857142857143" customWidth="1"/>
+    <col min="13" max="13" width="26" customWidth="1"/>
+    <col min="14" max="14" width="25.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2">
+        <v>2020</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" s="2">
+        <v>9966556655</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" display="mccbillemail@yopmail.com" tooltip="mailto:mccbillemail@yopmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes in TestData and Homepage
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="11196" windowHeight="4260"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="14700" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="123">
   <si>
     <t>SearchSKU</t>
   </si>
@@ -376,13 +376,25 @@
   </si>
   <si>
     <t>mccbillemail@yopmail.com</t>
+  </si>
+  <si>
+    <t>SingleSearch</t>
+  </si>
+  <si>
+    <t>BrandSearch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DEWALT-DCS331B</t>
+  </si>
+  <si>
+    <t>DeWalt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -427,6 +439,13 @@
       <name val="Arial"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.9"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -442,12 +461,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -459,7 +493,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -488,6 +522,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -835,61 +875,79 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.21875" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="D1" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="15">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="16" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="15">
         <v>1</v>
       </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="15">
         <v>2</v>
       </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="119" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="119" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Changes in the Homepage and Search
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="14700" windowHeight="7800"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="14700" windowHeight="4260"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="creditCardInfo" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:J13"/>
+  <oleSize ref="A1:L25"/>
 </workbook>
 </file>
 
@@ -384,10 +384,10 @@
     <t>BrandSearch</t>
   </si>
   <si>
-    <t xml:space="preserve"> DEWALT-DCS331B</t>
-  </si>
-  <si>
     <t>DeWalt</t>
+  </si>
+  <si>
+    <t>DEWALT-DCS331B</t>
   </si>
 </sst>
 </file>
@@ -875,7 +875,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -914,10 +914,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>121</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1466,7 +1466,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Shipping and Billing Page Scripts for the adhoc defects test design
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="14700" windowHeight="4260"/>
+    <workbookView windowWidth="20220" windowHeight="12150" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,15 @@
     <sheet name="MyAcc_PInfo" sheetId="3" r:id="rId3"/>
     <sheet name="addrBook" sheetId="4" r:id="rId4"/>
     <sheet name="creditCardInfo" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <oleSize ref="A1:L25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130">
   <si>
     <t>SearchSKU</t>
   </si>
@@ -30,12 +31,24 @@
     <t>InvalidSearch</t>
   </si>
   <si>
+    <t>SingleSearch</t>
+  </si>
+  <si>
+    <t>BrandSearch</t>
+  </si>
+  <si>
     <t>c280</t>
   </si>
   <si>
     <t>!@#$%^&amp;*()</t>
   </si>
   <si>
+    <t>DEWALT-DCS331B</t>
+  </si>
+  <si>
+    <t>DeWalt</t>
+  </si>
+  <si>
     <t>fluke</t>
   </si>
   <si>
@@ -60,7 +73,7 @@
     <t>Main Account with orders</t>
   </si>
   <si>
-    <t>acmeautomation1@yopmail.com</t>
+    <t>acmeautomation9@yopmail.com</t>
   </si>
   <si>
     <t>P@ssw0rd</t>
@@ -372,29 +385,44 @@
     <t>228 Park Ave S</t>
   </si>
   <si>
-    <t>verona</t>
+    <t>35011</t>
+  </si>
+  <si>
+    <t>alabama</t>
   </si>
   <si>
     <t>mccbillemail@yopmail.com</t>
   </si>
   <si>
-    <t>SingleSearch</t>
-  </si>
-  <si>
-    <t>BrandSearch</t>
-  </si>
-  <si>
-    <t>DeWalt</t>
-  </si>
-  <si>
-    <t>DEWALT-DCS331B</t>
+    <t>Billing details added in checkout to be saved to My Account</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>chkBillingfname</t>
+  </si>
+  <si>
+    <t>chkBillinglname</t>
+  </si>
+  <si>
+    <t>4772  Red Dog Road</t>
+  </si>
+  <si>
+    <t>chkBillingComp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -444,10 +472,153 @@
       <sz val="9.9"/>
       <color rgb="FF444444"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,8 +631,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -471,25 +828,264 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -508,32 +1104,79 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="10" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -866,24 +1509,24 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.78095238095238" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.2190476190476" customWidth="1"/>
+    <col min="3" max="3" width="11.7809523809524" customWidth="1"/>
+    <col min="4" max="4" width="18.2190476190476" customWidth="1"/>
+    <col min="5" max="5" width="16.2190476190476" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -897,32 +1540,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>120</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="15">
         <v>5</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" s="15">
         <v>1</v>
@@ -933,7 +1576,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="15" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" s="15">
         <v>2</v>
@@ -944,510 +1587,513 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" display="!@#$%^&amp;*()"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="119" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="119" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.78095238095238" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="53.44140625" customWidth="1"/>
+    <col min="1" max="1" width="27.4380952380952" customWidth="1"/>
+    <col min="2" max="2" width="28.7809523809524" customWidth="1"/>
+    <col min="3" max="3" width="10.7809523809524" customWidth="1"/>
+    <col min="4" max="4" width="53.4380952380952" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>18</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1" display="acmeautomation9@yopmail.com" tooltip="mailto:acmeautomation9@yopmail.com"/>
+    <hyperlink ref="B5" r:id="rId2" display="abooknoaddr@yopmail.com"/>
+    <hyperlink ref="B3" r:id="rId3" display="acmenoorders@yopmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.78095238095238" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" customWidth="1"/>
-    <col min="13" max="13" width="25.44140625" customWidth="1"/>
-    <col min="14" max="14" width="19.5546875" customWidth="1"/>
-    <col min="15" max="15" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.2190476190476" customWidth="1"/>
+    <col min="4" max="4" width="17.2190476190476" customWidth="1"/>
+    <col min="5" max="5" width="16.4380952380952" customWidth="1"/>
+    <col min="7" max="7" width="15.7809523809524" customWidth="1"/>
+    <col min="10" max="10" width="10.2190476190476" customWidth="1"/>
+    <col min="11" max="11" width="12.4380952380952" customWidth="1"/>
+    <col min="12" max="12" width="21.4380952380952" customWidth="1"/>
+    <col min="13" max="13" width="25.4380952380952" customWidth="1"/>
+    <col min="14" max="14" width="19.552380952381" customWidth="1"/>
+    <col min="15" max="15" width="15.7809523809524" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
       <c r="T1" s="8"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="N2">
         <v>9898989898</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="P2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="N3">
         <v>8877887788</v>
       </c>
       <c r="O3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="P3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="9:16">
       <c r="I4" s="9" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="O4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="P4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="9:16">
       <c r="I5" s="9" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="J5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="K5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="P5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="9:16">
       <c r="I6" s="9" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="P6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="9:16">
       <c r="I7" s="9" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="P7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="9:16">
       <c r="I8" s="9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="J8" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K8" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="P8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="9:16">
       <c r="I9" s="9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="K9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="P9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="9:16">
       <c r="I10" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J10" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K10" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="P10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="9:16">
       <c r="I11" s="9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="J11" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="K11" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="P11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="16:16">
       <c r="P12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="16:16">
       <c r="P13" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="M2" r:id="rId3"/>
-    <hyperlink ref="L2" r:id="rId4"/>
+    <hyperlink ref="M3" r:id="rId1" display="myacc_pinfoedit@yopmail.com"/>
+    <hyperlink ref="L3" r:id="rId1" display="myacc_pinfoedit@yopmail.com"/>
+    <hyperlink ref="M2" r:id="rId2" display="pinfoedited@yopmail.com"/>
+    <hyperlink ref="L2" r:id="rId2" display="pinfoedited@yopmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XEZ2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="23.3333333333333" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="16380" width="23.33203125" style="2" customWidth="1"/>
-    <col min="16381" max="16384" width="23.33203125" style="2"/>
+    <col min="1" max="16380" width="23.3333333333333" style="2" customWidth="1"/>
+    <col min="16381" max="16384" width="23.3333333333333" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" ht="28.8">
+    <row r="2" ht="30" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="L2" s="2">
         <v>5566556655</v>
@@ -1455,125 +2101,180 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" tooltip="mailto:newshipemail@yopmail.com"/>
+    <hyperlink ref="K2" r:id="rId1" display="newshipemail@yopmail.com" tooltip="mailto:newshipemail@yopmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.552380952381" customWidth="1"/>
+    <col min="2" max="2" width="19.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="19.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="13.4380952380952" customWidth="1"/>
+    <col min="6" max="6" width="16.552380952381" customWidth="1"/>
+    <col min="7" max="7" width="20.4380952380952" customWidth="1"/>
+    <col min="8" max="8" width="22.3333333333333" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
-    <col min="14" max="14" width="25.6640625" customWidth="1"/>
+    <col min="14" max="14" width="25.6666666666667" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="28.8">
+    </row>
+    <row r="2" ht="30" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>112</v>
+        <v>115</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>116</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E2">
         <v>2020</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="N2" s="2">
+        <v>8899889988</v>
+      </c>
+    </row>
+    <row r="3" ht="45" spans="1:15">
+      <c r="A3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="C3" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="N2" s="2">
-        <v>9966556655</v>
+      <c r="D3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3">
+        <v>2022</v>
+      </c>
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3">
+        <v>28202</v>
+      </c>
+      <c r="O3" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" tooltip="mailto:mccbillemail@yopmail.com"/>
+    <hyperlink ref="M2" r:id="rId1" display="mccbillemail@yopmail.com" tooltip="mailto:mccbillemail@yopmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes in the Category pages , PDP, Registeration, Checkout
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="14700" windowHeight="4260"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="14700" windowHeight="2448" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="creditCardInfo" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:L25"/>
+  <oleSize ref="A1:D7"/>
 </workbook>
 </file>
 
@@ -60,9 +60,6 @@
     <t>Main Account with orders</t>
   </si>
   <si>
-    <t>acmeautomation1@yopmail.com</t>
-  </si>
-  <si>
     <t>P@ssw0rd</t>
   </si>
   <si>
@@ -388,6 +385,9 @@
   </si>
   <si>
     <t>DEWALT-DCS331B</t>
+  </si>
+  <si>
+    <t>acmeautomation4@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -874,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -897,10 +897,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -914,10 +914,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -991,52 +991,52 @@
         <v>12</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1078,49 +1078,49 @@
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -1129,221 +1129,221 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="M2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N2">
         <v>9898989898</v>
       </c>
       <c r="O2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" t="s">
         <v>50</v>
-      </c>
-      <c r="P2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>54</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>55</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>56</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" t="s">
         <v>58</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>59</v>
       </c>
-      <c r="K3" t="s">
-        <v>60</v>
-      </c>
       <c r="L3" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N3">
         <v>8877887788</v>
       </c>
       <c r="O3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" t="s">
         <v>61</v>
-      </c>
-      <c r="P3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="I4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" t="s">
         <v>63</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>64</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
         <v>65</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>66</v>
-      </c>
-      <c r="P4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="I5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" t="s">
         <v>68</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>69</v>
       </c>
-      <c r="K5" t="s">
+      <c r="P5" t="s">
         <v>70</v>
-      </c>
-      <c r="P5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="I6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" t="s">
         <v>72</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>73</v>
       </c>
-      <c r="K6" t="s">
+      <c r="P6" t="s">
         <v>74</v>
-      </c>
-      <c r="P6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="I7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s">
         <v>76</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
+        <v>73</v>
+      </c>
+      <c r="P7" t="s">
         <v>77</v>
-      </c>
-      <c r="K7" t="s">
-        <v>74</v>
-      </c>
-      <c r="P7" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="I8" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" t="s">
         <v>79</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>80</v>
       </c>
-      <c r="K8" t="s">
+      <c r="P8" t="s">
         <v>81</v>
-      </c>
-      <c r="P8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="I9" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" t="s">
         <v>83</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>84</v>
       </c>
-      <c r="K9" t="s">
+      <c r="P9" t="s">
         <v>85</v>
-      </c>
-      <c r="P9" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="I10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" t="s">
         <v>87</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>88</v>
       </c>
-      <c r="K10" t="s">
+      <c r="P10" t="s">
         <v>89</v>
-      </c>
-      <c r="P10" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="I11" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" t="s">
         <v>91</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>92</v>
       </c>
-      <c r="K11" t="s">
+      <c r="P11" t="s">
         <v>93</v>
-      </c>
-      <c r="P11" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="P12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="P13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1378,37 +1378,37 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1417,37 +1417,37 @@
     </row>
     <row r="2" spans="1:16" ht="28.8">
       <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="L2" s="2">
         <v>5566556655</v>
@@ -1487,84 +1487,84 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="28.8">
       <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
         <v>110</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="E2">
         <v>2020</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="N2" s="2">
         <v>9966556655</v>

</xml_diff>

<commit_message>
changes in the shopping cart and shipping pages
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="14700" windowHeight="2448" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="14700" windowHeight="2448" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="creditCardInfo" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:D7"/>
+  <oleSize ref="G1:N6"/>
 </workbook>
 </file>
 
@@ -956,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1465,7 +1465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Guest order confirmation final and test data update
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="14700" windowHeight="2448" activeTab="4"/>
+    <workbookView windowWidth="20220" windowHeight="12150" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,13 @@
     <sheet name="addrBook" sheetId="4" r:id="rId4"/>
     <sheet name="creditCardInfo" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="G1:N6"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <oleSize ref="A1:H6"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128">
   <si>
     <t>SearchSKU</t>
   </si>
@@ -30,12 +30,24 @@
     <t>InvalidSearch</t>
   </si>
   <si>
+    <t>SingleSearch</t>
+  </si>
+  <si>
+    <t>BrandSearch</t>
+  </si>
+  <si>
     <t>c280</t>
   </si>
   <si>
     <t>!@#$%^&amp;*()</t>
   </si>
   <si>
+    <t>DEWALT-DCS331B</t>
+  </si>
+  <si>
+    <t>DeWalt</t>
+  </si>
+  <si>
     <t>fluke</t>
   </si>
   <si>
@@ -60,6 +72,9 @@
     <t>Main Account with orders</t>
   </si>
   <si>
+    <t>acmeautomation9@yopmail.com</t>
+  </si>
+  <si>
     <t>P@ssw0rd</t>
   </si>
   <si>
@@ -375,26 +390,32 @@
     <t>mccbillemail@yopmail.com</t>
   </si>
   <si>
-    <t>SingleSearch</t>
-  </si>
-  <si>
-    <t>BrandSearch</t>
-  </si>
-  <si>
-    <t>DeWalt</t>
-  </si>
-  <si>
-    <t>DEWALT-DCS331B</t>
-  </si>
-  <si>
-    <t>acmeautomation4@yopmail.com</t>
+    <t>05</t>
+  </si>
+  <si>
+    <t>billingchkfname</t>
+  </si>
+  <si>
+    <t>billingchklnmae</t>
+  </si>
+  <si>
+    <t>78 plaza drive</t>
+  </si>
+  <si>
+    <t>billingchk@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -444,10 +465,153 @@
       <sz val="9.9"/>
       <color rgb="FF444444"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,8 +624,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -471,25 +821,264 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -508,32 +1097,79 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="10" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -866,24 +1502,24 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.78095238095238" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.2190476190476" customWidth="1"/>
+    <col min="3" max="3" width="11.7809523809524" customWidth="1"/>
+    <col min="4" max="4" width="18.2190476190476" customWidth="1"/>
+    <col min="5" max="5" width="16.2190476190476" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -897,32 +1533,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>118</v>
+        <v>3</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>119</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="15">
         <v>5</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" s="15">
         <v>1</v>
@@ -933,7 +1569,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="15" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" s="15">
         <v>2</v>
@@ -944,510 +1580,514 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" display="!@#$%^&amp;*()"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="119" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="119" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.78095238095238" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="53.44140625" customWidth="1"/>
+    <col min="1" max="1" width="27.4380952380952" customWidth="1"/>
+    <col min="2" max="2" width="28.7809523809524" customWidth="1"/>
+    <col min="3" max="3" width="10.7809523809524" customWidth="1"/>
+    <col min="4" max="4" width="53.4380952380952" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>11</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>16</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1" display="acmeautomation9@yopmail.com" tooltip="mailto:acmeautomation9@yopmail.com"/>
+    <hyperlink ref="B5" r:id="rId2" display="abooknoaddr@yopmail.com"/>
+    <hyperlink ref="B3" r:id="rId3" display="acmenoorders@yopmail.com"/>
+    <hyperlink ref="C2" r:id="rId4" display="P@ssw0rd"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.78095238095238" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" customWidth="1"/>
-    <col min="13" max="13" width="25.44140625" customWidth="1"/>
-    <col min="14" max="14" width="19.5546875" customWidth="1"/>
-    <col min="15" max="15" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.2190476190476" customWidth="1"/>
+    <col min="4" max="4" width="17.2190476190476" customWidth="1"/>
+    <col min="5" max="5" width="16.4380952380952" customWidth="1"/>
+    <col min="7" max="7" width="15.7809523809524" customWidth="1"/>
+    <col min="10" max="10" width="10.2190476190476" customWidth="1"/>
+    <col min="11" max="11" width="12.4380952380952" customWidth="1"/>
+    <col min="12" max="12" width="21.4380952380952" customWidth="1"/>
+    <col min="13" max="13" width="25.4380952380952" customWidth="1"/>
+    <col min="14" max="14" width="19.552380952381" customWidth="1"/>
+    <col min="15" max="15" width="15.7809523809524" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="L1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>48</v>
+        <v>52</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="N2">
         <v>9898989898</v>
       </c>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>57</v>
+        <v>61</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>20</v>
+        <v>64</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="N3">
         <v>8877887788</v>
       </c>
       <c r="O3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="P3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="I4" s="9" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="9:16">
+      <c r="I4" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="O4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="P4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="I5" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="9:16">
+      <c r="I5" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="J5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="K5" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="P5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="I6" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="9:16">
+      <c r="I6" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="P6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="I7" s="9" t="s">
-        <v>75</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="9:16">
+      <c r="I7" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="K7" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="P7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="I8" s="9" t="s">
-        <v>78</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="9:16">
+      <c r="I8" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="J8" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="K8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="P8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="I9" s="9" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="9:16">
+      <c r="I9" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="K9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="P9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="I10" s="9" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="9:16">
+      <c r="I10" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="J10" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="K10" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="P10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="I11" s="9" t="s">
-        <v>90</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="9:16">
+      <c r="I11" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="J11" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="K11" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="P11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="16:16">
       <c r="P12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="16:16">
       <c r="P13" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="M2" r:id="rId3"/>
-    <hyperlink ref="L2" r:id="rId4"/>
+    <hyperlink ref="M3" r:id="rId1" display="myacc_pinfoedit@yopmail.com"/>
+    <hyperlink ref="L3" r:id="rId1" display="myacc_pinfoedit@yopmail.com"/>
+    <hyperlink ref="M2" r:id="rId2" display="pinfoedited@yopmail.com"/>
+    <hyperlink ref="L2" r:id="rId2" display="pinfoedited@yopmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XEZ2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="23.3333333333333" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="16380" width="23.33203125" style="2" customWidth="1"/>
-    <col min="16381" max="16384" width="23.33203125" style="2"/>
+    <col min="1" max="16380" width="23.3333333333333" style="2" customWidth="1"/>
+    <col min="16381" max="16384" width="23.3333333333333" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" ht="28.8">
+    <row r="2" ht="30" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>104</v>
+        <v>69</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="L2" s="2">
         <v>5566556655</v>
@@ -1455,125 +2095,170 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" tooltip="mailto:newshipemail@yopmail.com"/>
+    <hyperlink ref="K2" r:id="rId1" display="newshipemail@yopmail.com" tooltip="mailto:newshipemail@yopmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.552380952381" customWidth="1"/>
+    <col min="2" max="2" width="19.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="19.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="13.4380952380952" customWidth="1"/>
+    <col min="6" max="6" width="16.552380952381" customWidth="1"/>
+    <col min="7" max="7" width="20.4380952380952" customWidth="1"/>
+    <col min="8" max="8" width="22.3333333333333" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
-    <col min="14" max="14" width="25.6640625" customWidth="1"/>
+    <col min="14" max="14" width="25.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="28.8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>116</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E2">
         <v>2020</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="N2" s="2">
         <v>9966556655</v>
       </c>
     </row>
+    <row r="3" spans="2:14">
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3">
+        <v>2025</v>
+      </c>
+      <c r="F3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3">
+        <v>35010</v>
+      </c>
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="N3">
+        <v>9988998899</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" tooltip="mailto:mccbillemail@yopmail.com"/>
+    <hyperlink ref="M2" r:id="rId1" display="mccbillemail@yopmail.com" tooltip="mailto:mccbillemail@yopmail.com"/>
+    <hyperlink ref="M3" r:id="rId2" display="billingchk@yopmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes in the reusables
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="13104" windowHeight="4380" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="13104" windowHeight="4380"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="127">
   <si>
     <t>SearchSKU</t>
   </si>
@@ -396,6 +396,9 @@
   </si>
   <si>
     <t>qaacme</t>
+  </si>
+  <si>
+    <t>Bopis</t>
   </si>
 </sst>
 </file>
@@ -892,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -906,7 +909,7 @@
     <col min="5" max="5" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -922,8 +925,11 @@
       <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
@@ -939,8 +945,11 @@
       <c r="E2" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="14">
+        <v>58102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="14" t="s">
         <v>9</v>
       </c>
@@ -950,8 +959,9 @@
       <c r="C3" s="14"/>
       <c r="D3" s="16"/>
       <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
@@ -961,6 +971,7 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -976,7 +987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes in the checkout signup and removed cLP commented scripts
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="13104" windowHeight="4380"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="13104" windowHeight="4380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="129">
   <si>
     <t>SearchSKU</t>
   </si>
@@ -399,6 +399,12 @@
   </si>
   <si>
     <t>Bopis</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>testaccount@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -897,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -985,10 +991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -998,9 +1004,10 @@
     <col min="3" max="3" width="10.77734375" customWidth="1"/>
     <col min="4" max="4" width="53.44140625" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1016,8 +1023,11 @@
       <c r="E1" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1033,8 +1043,11 @@
       <c r="E2" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1048,7 +1061,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1059,7 +1072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Changes in the failures
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
   <si>
     <t>SearchSKU</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>testaccount@yopmail.com</t>
+  </si>
+  <si>
+    <t>acmeqa1</t>
   </si>
 </sst>
 </file>
@@ -993,13 +996,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="51.44140625" customWidth="1"/>
     <col min="2" max="2" width="28.77734375" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" customWidth="1"/>
     <col min="4" max="4" width="53.44140625" customWidth="1"/>
@@ -1052,7 +1055,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -1077,7 +1080,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -1087,11 +1090,9 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2" display="mailto:acmeautomation2@yopmail.com%0a"/>
-    <hyperlink ref="B3" r:id="rId3" display="mailto:acmeautomation1@yopmail.com"/>
-    <hyperlink ref="B5" r:id="rId4" display="mailto:acmeautomation1@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -1106,7 +1107,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
+    <col min="1" max="1" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.21875" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" customWidth="1"/>
     <col min="7" max="7" width="15.77734375" customWidth="1"/>

</xml_diff>

<commit_message>
Scripts included RequestQuote, RequisitionList, Catalog
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="136">
   <si>
     <t>SearchSKU</t>
   </si>
@@ -408,6 +408,24 @@
   </si>
   <si>
     <t>acmeqa1</t>
+  </si>
+  <si>
+    <t>B2BUsername</t>
+  </si>
+  <si>
+    <t>B2BPassword</t>
+  </si>
+  <si>
+    <t>businessuse1</t>
+  </si>
+  <si>
+    <t>GOUsername</t>
+  </si>
+  <si>
+    <t>GOPassword</t>
+  </si>
+  <si>
+    <t>govern1</t>
   </si>
 </sst>
 </file>
@@ -994,23 +1012,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="53.44140625" customWidth="1"/>
-    <col min="5" max="5" width="49" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1021,16 +1042,28 @@
         <v>13</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1040,17 +1073,29 @@
       <c r="C2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1060,11 +1105,11 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1075,7 +1120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Changes in the Organization and Buyer
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="13104" windowHeight="4380" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="14988" windowHeight="2532" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="creditCardInfo" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -1015,7 +1016,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1452,7 +1453,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:XEZ2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>

</xml_diff>